<commit_message>
didn't commit over the last few days. started agenda_main2.py to include saving and loading agendas to .txt file but I think I should have left the original/ver1 to be fully functional from the command line and forked a new version
</commit_message>
<xml_diff>
--- a/Agenda1.xlsx
+++ b/Agenda1.xlsx
@@ -450,7 +450,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -475,7 +475,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -500,7 +500,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -550,7 +550,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -575,7 +575,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -600,7 +600,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -650,7 +650,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -675,7 +675,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>

</xml_diff>